<commit_message>
aktualizacja pozostalych zadan w rejestrze sprintu
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -2,26 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="60" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Opis" sheetId="3" r:id="rId1"/>
-    <sheet name="Rejestr Produktu" sheetId="1" r:id="rId2"/>
-    <sheet name="Rejestr Sprint #1" sheetId="2" r:id="rId3"/>
+    <sheet name="Opis" sheetId="1" r:id="rId1"/>
+    <sheet name="Rejestr Produktu" sheetId="2" r:id="rId2"/>
+    <sheet name="Rejestr Sprint #1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+  <si>
+    <t>Text Transformer</t>
+  </si>
+  <si>
+    <t>Dla osób pracujących z danymi tekstowymi nasza aplikacja Text Transformer umożliwi transformacje danych tekstowych (np. zmiana wielkości liter, eliminacja duplikatów, itd.). Aplikacja będzie dostępna poprzez GUI a także zdalne API dzięki czemu będzie można ją zintegrować z istniejącymi narzędziami.</t>
+  </si>
   <si>
     <t>Element rejestru produktu</t>
   </si>
@@ -32,13 +38,10 @@
     <t>Pracochłonność</t>
   </si>
   <si>
+    <t>Business Value (BV)</t>
+  </si>
+  <si>
     <t>Kryteria akceptacji</t>
-  </si>
-  <si>
-    <t>Text Transformer</t>
-  </si>
-  <si>
-    <t>Dla osób pracujących z danymi tekstowymi nasza aplikacja Text Transformer umożliwi transformacje danych tekstowych (np. zmiana wielkości liter, eliminacja duplikatów, itd.). Aplikacja będzie dostępna poprzez GUI a także zdalne API dzięki czemu będzie można ją zintegrować z istniejącymi narzędziami.</t>
   </si>
   <si>
     <t>Jako twórca aplikacji mogę wywołać transformację zdalnie poprzez REST, aby móc  zintegrować narzędzie z moimi innymi aplikacjami</t>
@@ -66,9 +69,6 @@
 • Odwrócenie ciągu znaków
 • Wsparcie dla wszystkich znaków UTF-8
 </t>
-  </si>
-  <si>
-    <t>Business Value (BV)</t>
   </si>
   <si>
     <t>Jako użytkownik mogę zamieniać liczby na tekst w języku polskim (Wpłać 100 złotych -&gt; wpłać sto złotych) – wsparcie zakresu liczb do negocjacji</t>
@@ -123,58 +123,60 @@
     <t>Do późniejszej negocjacji</t>
   </si>
   <si>
+    <t>Cel sprintu:</t>
+  </si>
+  <si>
     <t>Zadania</t>
   </si>
   <si>
-    <t>Element przekopiowany z zakładki Rejestr Produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 1 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 2 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 3 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 4 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pracochłonność </t>
   </si>
   <si>
-    <t>(dla elementu rejestru produktu)</t>
-  </si>
-  <si>
-    <t>(dla zadania)</t>
-  </si>
-  <si>
-    <t>Cel sprintu:</t>
+    <t>utworzenie podstawowej wersji aplikacji do transformacji tekstu z interfejsem RESTowym</t>
+  </si>
+  <si>
+    <t>• Skonfigurowanie interfejsu REST</t>
+  </si>
+  <si>
+    <t>• Implementacja klasy Inverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Implementacja klasy BasicTransforms
+</t>
+  </si>
+  <si>
+    <t>• Implementacja klasy NumbersExpander</t>
+  </si>
+  <si>
+    <t>• Implementacja klasy ShortcutsModifier</t>
+  </si>
+  <si>
+    <t>• Implementacja klasy LatexCharacters</t>
+  </si>
+  <si>
+    <t>• Implementacja klasy NeighborsRemover</t>
+  </si>
+  <si>
+    <t>• Implementacja aplikacji konsolowej</t>
+  </si>
+  <si>
+    <t>Pozostałe</t>
+  </si>
+  <si>
+    <t>zapoznanie się z technologią niezbędną do wykonania projektu, utworzenie i skonfigurowanie repozytorium git, skonfigurowanie środowiska ciągłej integracji (travis), skonfigurowanie środowiska do zarządzania (trello), skonfigurowanie narzędzia automatyzującego budowę oprogramowania (maven), napisanie README</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -182,32 +184,28 @@
       <color rgb="FF4F81BD"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,36 +225,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -264,92 +242,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
-    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="19" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="20" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -359,35 +340,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E10" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Element rejestru produktu" dataDxfId="8"/>
-    <tableColumn id="2" name="Ważność" dataDxfId="7"/>
-    <tableColumn id="3" name="Pracochłonność" dataDxfId="6"/>
-    <tableColumn id="4" name="Business Value (BV)" dataDxfId="5"/>
-    <tableColumn id="5" name="Kryteria akceptacji" dataDxfId="4"/>
+    <tableColumn id="1" name="Element rejestru produktu"/>
+    <tableColumn id="2" name="Ważność"/>
+    <tableColumn id="3" name="Pracochłonność"/>
+    <tableColumn id="4" name="Business Value (BV)"/>
+    <tableColumn id="5" name="Kryteria akceptacji"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:C44" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A4:C44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela3" displayName="Tabela3" ref="A4:C14" totalsRowShown="0">
+  <autoFilter ref="A4:C14"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Element rejestru produktu" dataDxfId="2"/>
-    <tableColumn id="2" name="Zadania" dataDxfId="1"/>
-    <tableColumn id="3" name="Pracochłonność " dataDxfId="0"/>
+    <tableColumn id="1" name="Element rejestru produktu"/>
+    <tableColumn id="2" name="Zadania"/>
+    <tableColumn id="3" name="Pracochłonność "/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -425,7 +406,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -497,7 +478,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,16 +510,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -660,46 +645,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -708,32 +654,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.5" customWidth="1"/>
+    <col min="1" max="1" width="97.875"/>
+    <col min="2" max="1025" width="10.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -741,262 +682,347 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="53.25" style="3"/>
+    <col min="2" max="2" width="15.375" style="4"/>
+    <col min="3" max="3" width="22.25" style="4"/>
+    <col min="4" max="4" width="25.875" style="4"/>
+    <col min="5" max="5" width="59.625" style="3"/>
+    <col min="6" max="1025" width="10.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
+      <c r="A2" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>15</v>
       </c>
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
+      <c r="A3" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="4">
         <v>12</v>
       </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
       <c r="D3" s="4">
         <v>0.5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
+      <c r="A4" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="4">
         <v>10</v>
       </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
       <c r="D4" s="4">
         <v>0.5</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>10</v>
       </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4">
         <v>10</v>
       </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
       <c r="D6" s="4">
         <v>0.5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="4">
         <v>10</v>
       </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
       <c r="D7" s="4">
         <v>0.5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
       </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
       <c r="D8" s="4">
         <v>0.5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
       </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33" style="4" customWidth="1"/>
+    <col min="1" max="1" width="46.375" style="7"/>
+    <col min="2" max="2" width="50" style="7"/>
+    <col min="3" max="3" width="33.75" style="4"/>
+    <col min="4" max="1025" width="10.625"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1"/>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>31</v>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zaktualizowano zadania do sprintu #2
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Text Transformer</t>
   </si>
@@ -165,12 +165,24 @@
   <si>
     <t>zapoznanie się z technologią niezbędną do wykonania projektu, utworzenie i skonfigurowanie repozytorium git, skonfigurowanie środowiska ciągłej integracji (travis), skonfigurowanie środowiska do zarządzania (trello), skonfigurowanie narzędzia automatyzującego budowę oprogramowania (maven), napisanie README</t>
   </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Jako użytkownik mogę przekształcić tekst tak, aby posiadał znaki interpunkcyjne w odpowiednich miejscach (np. Myślę że tak Albo jednak nie -&gt; Myślę,  że tak. Albo jednak nie.)</t>
+  </si>
+  <si>
+    <t>Jako użytkownik mogę zmieniać tekst na leetspeak (leetspeak -&gt; 1337sp34k)</t>
+  </si>
+  <si>
+    <t>Jako użytkownik mogę usunąć polskie znaki z tekstu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -207,6 +219,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -255,6 +275,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,10 +703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -860,6 +883,29 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -871,10 +917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A16:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1018,6 +1064,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>